<commit_message>
vegetation up to 1950, confinement cells and PEST set-up
</commit_message>
<xml_diff>
--- a/Data/data_waterlevels/obs/06_Steady_state_groundwater_obs.xlsx
+++ b/Data/data_waterlevels/obs/06_Steady_state_groundwater_obs.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -513,6 +513,11 @@
           <t>Sample timeframe</t>
         </is>
       </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>model_timestamp</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -564,6 +569,9 @@
           <t>1969_Wet</t>
         </is>
       </c>
+      <c r="P2" t="n">
+        <v>6993</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -615,6 +623,9 @@
           <t>1969_Wet</t>
         </is>
       </c>
+      <c r="P3" t="n">
+        <v>6993</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -664,6 +675,9 @@
           <t>1969_Wet</t>
         </is>
       </c>
+      <c r="P4" t="n">
+        <v>6993</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -715,6 +729,9 @@
           <t>1969_Wet</t>
         </is>
       </c>
+      <c r="P5" t="n">
+        <v>6993</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -764,6 +781,9 @@
           <t>1969_Wet</t>
         </is>
       </c>
+      <c r="P6" t="n">
+        <v>6993</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -813,6 +833,9 @@
           <t>1969_Wet</t>
         </is>
       </c>
+      <c r="P7" t="n">
+        <v>6993</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -864,6 +887,9 @@
           <t>1969_Wet</t>
         </is>
       </c>
+      <c r="P8" t="n">
+        <v>6993</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -915,6 +941,9 @@
           <t>1969_Wet</t>
         </is>
       </c>
+      <c r="P9" t="n">
+        <v>6993</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -966,6 +995,9 @@
           <t>1969_Wet</t>
         </is>
       </c>
+      <c r="P10" t="n">
+        <v>6993</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1017,6 +1049,9 @@
           <t>1969_Wet</t>
         </is>
       </c>
+      <c r="P11" t="n">
+        <v>6993</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1068,6 +1103,9 @@
           <t>1969_Wet</t>
         </is>
       </c>
+      <c r="P12" t="n">
+        <v>6993</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1118,6 +1156,9 @@
         <is>
           <t>1969_Wet</t>
         </is>
+      </c>
+      <c r="P13" t="n">
+        <v>6993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>